<commit_message>
Updated on 12-26 at 1441
</commit_message>
<xml_diff>
--- a/Settings.xlsx
+++ b/Settings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>Speeds and Powers for the ULS VLS2.30</t>
   </si>
@@ -59,7 +59,31 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Metal</t>
+    <t>Metal (mark only)</t>
+  </si>
+  <si>
+    <t>Scrapbook Paper</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>Quilted Glass</t>
+  </si>
+  <si>
+    <t>Z-Axis</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>Hardboard</t>
+  </si>
+  <si>
+    <t>Birch Ply</t>
+  </si>
+  <si>
+    <t>Glass (Soda Ash)</t>
   </si>
 </sst>
 </file>
@@ -440,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +475,7 @@
     <col min="1" max="1" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -464,7 +488,7 @@
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -475,13 +499,13 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -495,26 +519,35 @@
       <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="N4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P4" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
@@ -529,55 +562,55 @@
         <v>500</v>
       </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="9">
+      <c r="H5" s="9">
         <v>45</v>
       </c>
-      <c r="H5" s="9">
+      <c r="I5" s="9">
         <v>10</v>
       </c>
-      <c r="I5" s="9">
+      <c r="J5" s="9">
         <v>500</v>
-      </c>
-      <c r="K5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" t="s">
-        <v>10</v>
       </c>
       <c r="M5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>95</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>3.8</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -589,6 +622,148 @@
       </c>
       <c r="E10">
         <v>600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11">
+        <v>26.1</v>
+      </c>
+      <c r="I11">
+        <v>15</v>
+      </c>
+      <c r="J11">
+        <v>500</v>
+      </c>
+      <c r="K11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12">
+        <v>30</v>
+      </c>
+      <c r="N12">
+        <v>19</v>
+      </c>
+      <c r="O12">
+        <v>165</v>
+      </c>
+      <c r="P12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
+      </c>
+      <c r="D13">
+        <v>3.75</v>
+      </c>
+      <c r="E13">
+        <v>600</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13">
+        <v>100</v>
+      </c>
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <v>600</v>
+      </c>
+      <c r="K13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13">
+        <v>100</v>
+      </c>
+      <c r="N13">
+        <v>3.75</v>
+      </c>
+      <c r="O13">
+        <v>600</v>
+      </c>
+      <c r="P13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>100</v>
+      </c>
+      <c r="D17">
+        <v>70</v>
+      </c>
+      <c r="E17">
+        <v>500</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17">
+        <v>100</v>
+      </c>
+      <c r="I17">
+        <v>2.5</v>
+      </c>
+      <c r="J17">
+        <v>600</v>
+      </c>
+      <c r="K17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+      <c r="D18">
+        <v>53</v>
+      </c>
+      <c r="E18">
+        <v>500</v>
+      </c>
+      <c r="M18">
+        <v>30</v>
+      </c>
+      <c r="N18">
+        <v>19</v>
+      </c>
+      <c r="O18">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>